<commit_message>
Add Curve Prep - Ramer Douglas Peucker
</commit_message>
<xml_diff>
--- a/assets/Filtered_RDP.xlsx
+++ b/assets/Filtered_RDP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,417 +455,297 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.7900000000000006</v>
+        <v>1.51999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>3.793439660719471</v>
+        <v>3.866570477004245</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.51999999999999</v>
+        <v>2.824999999999962</v>
       </c>
       <c r="B4" t="n">
-        <v>3.866570477004245</v>
+        <v>4.04869366433339</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2.194999999999975</v>
+        <v>3.419999999999949</v>
       </c>
       <c r="B5" t="n">
-        <v>3.951262056579775</v>
+        <v>4.160676179989118</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2.824999999999962</v>
+        <v>3.974999999999937</v>
       </c>
       <c r="B6" t="n">
-        <v>4.04869366433339</v>
+        <v>4.286268202072216</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3.419999999999949</v>
+        <v>4.499999999999926</v>
       </c>
       <c r="B7" t="n">
-        <v>4.160676179989118</v>
+        <v>4.427522687840675</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3.974999999999937</v>
+        <v>4.994999999999916</v>
       </c>
       <c r="B8" t="n">
-        <v>4.286268202072216</v>
+        <v>4.584352985095669</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4.499999999999926</v>
+        <v>5.469999999999906</v>
       </c>
       <c r="B9" t="n">
-        <v>4.427522687840675</v>
+        <v>4.760151428656965</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4.994999999999916</v>
+        <v>5.924999999999896</v>
       </c>
       <c r="B10" t="n">
-        <v>4.584352985095669</v>
+        <v>4.955590221172241</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5.469999999999906</v>
+        <v>6.354999999999887</v>
       </c>
       <c r="B11" t="n">
-        <v>4.760151428656965</v>
+        <v>5.168383039921962</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5.924999999999896</v>
+        <v>6.769999999999878</v>
       </c>
       <c r="B12" t="n">
-        <v>4.955590221172241</v>
+        <v>5.403448912235375</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6.354999999999887</v>
+        <v>7.169999999999869</v>
       </c>
       <c r="B13" t="n">
-        <v>5.168383039921962</v>
+        <v>5.661478399030747</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6.769999999999878</v>
+        <v>7.549999999999861</v>
       </c>
       <c r="B14" t="n">
-        <v>5.403448912235375</v>
+        <v>5.938993691433978</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7.169999999999869</v>
+        <v>7.914999999999853</v>
       </c>
       <c r="B15" t="n">
-        <v>5.661478399030747</v>
+        <v>6.238970121890022</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7.549999999999861</v>
+        <v>8.269999999999893</v>
       </c>
       <c r="B16" t="n">
-        <v>5.938993691433978</v>
+        <v>6.565813901869458</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>7.914999999999853</v>
+        <v>8.56999999999994</v>
       </c>
       <c r="B17" t="n">
-        <v>6.238970121890022</v>
+        <v>6.871825224553957</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8.269999999999893</v>
+        <v>8.864999999999986</v>
       </c>
       <c r="B18" t="n">
-        <v>6.565813901869458</v>
+        <v>7.20185810163087</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8.56999999999994</v>
+        <v>9.435000000000075</v>
       </c>
       <c r="B19" t="n">
-        <v>6.871825224553957</v>
+        <v>7.93028933733765</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>8.864999999999986</v>
+        <v>9.98000000000016</v>
       </c>
       <c r="B20" t="n">
-        <v>7.20185810163087</v>
+        <v>8.751647504141467</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>9.155000000000031</v>
+        <v>10.51500000000024</v>
       </c>
       <c r="B21" t="n">
-        <v>7.556775782378767</v>
+        <v>9.68862540797388</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>9.435000000000075</v>
+        <v>10.96000000000031</v>
       </c>
       <c r="B22" t="n">
-        <v>7.93028933733765</v>
+        <v>10.5700353374158</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>9.710000000000118</v>
+        <v>11.42000000000039</v>
       </c>
       <c r="B23" t="n">
-        <v>8.328581477086036</v>
+        <v>11.57313703152733</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>9.98000000000016</v>
+        <v>12.71000000000059</v>
       </c>
       <c r="B24" t="n">
-        <v>8.751647504141467</v>
+        <v>14.66317533531265</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>10.2500000000002</v>
+        <v>13.09500000000065</v>
       </c>
       <c r="B25" t="n">
-        <v>9.207817189076302</v>
+        <v>15.54858902832022</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>10.51500000000024</v>
+        <v>13.4550000000007</v>
       </c>
       <c r="B26" t="n">
-        <v>9.68862540797388</v>
+        <v>16.30434783278508</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>10.73500000000028</v>
+        <v>13.79000000000076</v>
       </c>
       <c r="B27" t="n">
-        <v>10.11289159337599</v>
+        <v>16.92407118404208</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>10.96000000000031</v>
+        <v>14.14500000000081</v>
       </c>
       <c r="B28" t="n">
-        <v>10.5700353374158</v>
+        <v>17.480983440572</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>11.42000000000039</v>
+        <v>14.50500000000087</v>
       </c>
       <c r="B29" t="n">
-        <v>11.57313703152733</v>
+        <v>17.9392077909976</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>11.84000000000045</v>
+        <v>14.88000000000093</v>
       </c>
       <c r="B30" t="n">
-        <v>12.55555872957375</v>
+        <v>18.31075450709093</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>12.71000000000059</v>
+        <v>15.28000000000099</v>
       </c>
       <c r="B31" t="n">
-        <v>14.66317533531265</v>
+        <v>18.60540904374994</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>13.09500000000065</v>
+        <v>15.50500000000102</v>
       </c>
       <c r="B32" t="n">
-        <v>15.54858902832022</v>
+        <v>18.73302325580662</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>13.4550000000007</v>
+        <v>15.74000000000106</v>
       </c>
       <c r="B33" t="n">
-        <v>16.30434783278508</v>
+        <v>18.8421986466483</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>13.62500000000073</v>
+        <v>16.26000000000105</v>
       </c>
       <c r="B34" t="n">
-        <v>16.62981196852295</v>
+        <v>19.01524420676221</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>13.79000000000076</v>
+        <v>16.86500000000093</v>
       </c>
       <c r="B35" t="n">
-        <v>16.92407118404208</v>
+        <v>19.13443783186822</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>13.97000000000078</v>
+        <v>17.61500000000078</v>
       </c>
       <c r="B36" t="n">
-        <v>17.21962190797518</v>
+        <v>19.21165060099212</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>14.14500000000081</v>
+        <v>18.45500000000061</v>
       </c>
       <c r="B37" t="n">
-        <v>17.480983440572</v>
+        <v>19.25127425205064</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>14.32500000000084</v>
+        <v>19.61000000000038</v>
       </c>
       <c r="B38" t="n">
-        <v>17.72321562556372</v>
+        <v>19.27188538450635</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>14.50500000000087</v>
+        <v>24.99499999999931</v>
       </c>
       <c r="B39" t="n">
-        <v>17.9392077909976</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>14.6900000000009</v>
-      </c>
-      <c r="B40" t="n">
-        <v>18.13515846927362</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>14.88000000000093</v>
-      </c>
-      <c r="B41" t="n">
-        <v>18.31075450709093</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>15.07500000000096</v>
-      </c>
-      <c r="B42" t="n">
-        <v>18.46622776945848</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>15.28000000000099</v>
-      </c>
-      <c r="B43" t="n">
-        <v>18.60540904374994</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>15.50500000000102</v>
-      </c>
-      <c r="B44" t="n">
-        <v>18.73302325580662</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>15.74000000000106</v>
-      </c>
-      <c r="B45" t="n">
-        <v>18.8421986466483</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>15.9900000000011</v>
-      </c>
-      <c r="B46" t="n">
-        <v>18.9356971413481</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>16.26000000000105</v>
-      </c>
-      <c r="B47" t="n">
-        <v>19.01524420676221</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>16.55000000000099</v>
-      </c>
-      <c r="B48" t="n">
-        <v>19.08095570778583</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>16.86500000000093</v>
-      </c>
-      <c r="B49" t="n">
-        <v>19.13443783186822</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>17.22000000000086</v>
-      </c>
-      <c r="B50" t="n">
-        <v>19.17803511356391</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>17.61500000000078</v>
-      </c>
-      <c r="B51" t="n">
-        <v>19.21165060099212</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>18.45500000000061</v>
-      </c>
-      <c r="B52" t="n">
-        <v>19.25127425205064</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>19.61000000000038</v>
-      </c>
-      <c r="B53" t="n">
-        <v>19.27188538450635</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>24.99499999999931</v>
-      </c>
-      <c r="B54" t="n">
         <v>19.28122411429011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
calculate_curvature usando o np.gradient - melhoria de robustez
</commit_message>
<xml_diff>
--- a/assets/Filtered_RDP.xlsx
+++ b/assets/Filtered_RDP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,42 +447,458 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>20.17678</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>30.79460126660187</v>
+        <v>0.001984596919383877</v>
       </c>
       <c r="B3" t="n">
-        <v>0.01318042552552552</v>
+        <v>64.87384525750433</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>37.79655091322297</v>
+        <v>0.003868173634726945</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02589837997997998</v>
+        <v>76.85628397922264</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>39.00197108910267</v>
+        <v>0.006051410282056411</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0312167972972973</v>
+        <v>81.26546465228964</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>39.66155870212616</v>
+        <v>0.01001120224044809</v>
       </c>
       <c r="B6" t="n">
-        <v>0.042316103003003</v>
+        <v>85.06828772318971</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.01968593718743749</v>
+      </c>
+      <c r="B7" t="n">
+        <v>91.26443002797724</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.0250370074014803</v>
+      </c>
+      <c r="B8" t="n">
+        <v>93.08310049749753</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.02728445689137828</v>
+      </c>
+      <c r="B9" t="n">
+        <v>95.1610403112026</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.02959611922384477</v>
+      </c>
+      <c r="B10" t="n">
+        <v>95.38924286600356</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.03447629525905181</v>
+      </c>
+      <c r="B11" t="n">
+        <v>97.38972944328131</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.03650970194038808</v>
+      </c>
+      <c r="B12" t="n">
+        <v>97.55952273279601</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.04027685537107421</v>
+      </c>
+      <c r="B13" t="n">
+        <v>98.9448572254126</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.04209621924384876</v>
+      </c>
+      <c r="B14" t="n">
+        <v>98.60316176060762</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0.04408681736347269</v>
+      </c>
+      <c r="B15" t="n">
+        <v>99.71001229152353</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0.04449349869973995</v>
+      </c>
+      <c r="B16" t="n">
+        <v>99.73581373282001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.04549949989997999</v>
+      </c>
+      <c r="B17" t="n">
+        <v>99.65861097392623</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.04599179835967193</v>
+      </c>
+      <c r="B18" t="n">
+        <v>99.6895525034941</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.04993018603720744</v>
+      </c>
+      <c r="B19" t="n">
+        <v>100.7838227180577</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.05042248449689938</v>
+      </c>
+      <c r="B20" t="n">
+        <v>100.8236767534422</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.05149269853970794</v>
+      </c>
+      <c r="B21" t="n">
+        <v>100.7670245533888</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.05196359271854371</v>
+      </c>
+      <c r="B22" t="n">
+        <v>100.7899515108494</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0.05487457491498299</v>
+      </c>
+      <c r="B23" t="n">
+        <v>101.6072723156725</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.05513142628525705</v>
+      </c>
+      <c r="B24" t="n">
+        <v>101.6300382324279</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.05573074614922984</v>
+      </c>
+      <c r="B25" t="n">
+        <v>101.6062818875768</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0.0559875975195039</v>
+      </c>
+      <c r="B26" t="n">
+        <v>101.6216106563779</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0.05703640728145629</v>
+      </c>
+      <c r="B27" t="n">
+        <v>101.9036968261809</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.05776415283056611</v>
+      </c>
+      <c r="B28" t="n">
+        <v>101.8831463939445</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.05797819563912782</v>
+      </c>
+      <c r="B29" t="n">
+        <v>101.8962756656992</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.0589627925585117</v>
+      </c>
+      <c r="B30" t="n">
+        <v>102.172521258124</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.05988317663532707</v>
+      </c>
+      <c r="B31" t="n">
+        <v>102.1385558048806</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.06159551910382076</v>
+      </c>
+      <c r="B32" t="n">
+        <v>103.2758473949729</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0.06324364872974594</v>
+      </c>
+      <c r="B33" t="n">
+        <v>102.9763586476114</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0.06429245849169833</v>
+      </c>
+      <c r="B34" t="n">
+        <v>103.0108921517697</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.06502020404080816</v>
+      </c>
+      <c r="B35" t="n">
+        <v>103.0038393554248</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.06583356671334266</v>
+      </c>
+      <c r="B36" t="n">
+        <v>103.0076617985294</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.06660412082416484</v>
+      </c>
+      <c r="B37" t="n">
+        <v>102.9810334044963</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.0669251850370074</v>
+      </c>
+      <c r="B38" t="n">
+        <v>102.9949831539166</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.07092778555711142</v>
+      </c>
+      <c r="B39" t="n">
+        <v>104.0970692338103</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.07139867973594718</v>
+      </c>
+      <c r="B40" t="n">
+        <v>104.1320418188029</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0.07227625525105021</v>
+      </c>
+      <c r="B41" t="n">
+        <v>104.1011311515488</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.07362472494498899</v>
+      </c>
+      <c r="B42" t="n">
+        <v>104.117939449797</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0.07454510902180436</v>
+      </c>
+      <c r="B43" t="n">
+        <v>104.077236326668</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.0748875775155031</v>
+      </c>
+      <c r="B44" t="n">
+        <v>104.0912044814027</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.08019583916783356</v>
+      </c>
+      <c r="B45" t="n">
+        <v>105.2317132624075</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.08137307461492298</v>
+      </c>
+      <c r="B46" t="n">
+        <v>105.2061595148771</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.08235767153430686</v>
+      </c>
+      <c r="B47" t="n">
+        <v>105.2143336021544</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.08334226845369073</v>
+      </c>
+      <c r="B48" t="n">
+        <v>105.2121522882839</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0.08770874174834967</v>
+      </c>
+      <c r="B49" t="n">
+        <v>105.2131183810803</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0.08869333866773355</v>
+      </c>
+      <c r="B50" t="n">
+        <v>105.2106788889844</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0.08967793558711742</v>
+      </c>
+      <c r="B51" t="n">
+        <v>105.2199046177534</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0.09070534106821364</v>
+      </c>
+      <c r="B52" t="n">
+        <v>105.1860151445006</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0.09248189637927585</v>
+      </c>
+      <c r="B53" t="n">
+        <v>105.5426264095507</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0.09427985597119423</v>
+      </c>
+      <c r="B54" t="n">
+        <v>105.1738623574632</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0.09575675135027005</v>
+      </c>
+      <c r="B55" t="n">
+        <v>105.2915149021277</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0.09862492498499699</v>
+      </c>
+      <c r="B56" t="n">
+        <v>103.7276165515901</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0.1007225445089018</v>
+      </c>
+      <c r="B57" t="n">
+        <v>100.5547864362607</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="B58" t="n">
+        <v>76.77531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>